<commit_message>
Playing with Python std dev. Strange behaviour with checking for 2Sigma from average
</commit_message>
<xml_diff>
--- a/GeneticProgrammingPortfolio/sheets/ensemble-learning.xlsx
+++ b/GeneticProgrammingPortfolio/sheets/ensemble-learning.xlsx
@@ -618,7 +618,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="2"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -4346,7 +4346,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U28" sqref="U28"/>
+      <selection activeCell="U11" sqref="U11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
modified some .png and spreadsheets for outlier images
</commit_message>
<xml_diff>
--- a/GeneticProgrammingPortfolio/sheets/ensemble-learning.xlsx
+++ b/GeneticProgrammingPortfolio/sheets/ensemble-learning.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>Dow Jones</t>
   </si>
@@ -36,20 +36,23 @@
     <t>Best_Verification</t>
   </si>
   <si>
-    <t>Ensemble_Avg</t>
+    <t>Avg</t>
   </si>
   <si>
-    <t>Ensemble_Min</t>
+    <t>Max</t>
   </si>
   <si>
-    <t>Ensemble_Max</t>
+    <t>Min</t>
+  </si>
+  <si>
+    <t>Green uses outlier detection</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -57,13 +60,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -78,9 +99,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -133,11 +156,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-CA"/>
-              <a:t>Ensemble Approach, Min,</a:t>
+              <a:t>Ensemble Testing</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-CA" baseline="0"/>
-              <a:t> Max, and Avg</a:t>
+              <a:t> Without Outlier Detection</a:t>
             </a:r>
             <a:endParaRPr lang="en-CA"/>
           </a:p>
@@ -316,7 +339,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ensemble_Avg</c:v>
+                  <c:v>Avg</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -324,9 +347,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent2">
-                  <a:alpha val="20000"/>
-                </a:schemeClr>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -334,7 +355,7 @@
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="4"/>
             <c:spPr>
               <a:solidFill>
                 <a:schemeClr val="tx1"/>
@@ -457,7 +478,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ensemble_Max</c:v>
+                  <c:v>Max</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -600,7 +621,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Ensemble_Min</c:v>
+                  <c:v>Min</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -815,7 +836,7 @@
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1.1000000000000001"/>
-          <c:min val="0.60000000000000009"/>
+          <c:min val="0.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -944,7 +965,893 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-CA"/>
+              <a:t>Ensemble Testing With</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-CA" baseline="0"/>
+              <a:t> Outlier Detection</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-CA"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$A$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Dow Jones</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$A$256:$A$284</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.91423574600000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.90082181500000003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88898699400000003</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.90907392899999995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.88326484900000002</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.878408666</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.94187862899999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.93214928500000005</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.90046524299999997</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.90875131600000003</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.87526742999999996</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.84062892700000003</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.80069277000000005</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.840645906</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.89691649399999995</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.88774747899999995</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.86098753699999997</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.90881923499999995</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.91413386799999996</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.838183856</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.84893197899999995</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.85468808399999996</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.86777939999999998</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.90944748200000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.94223520199999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.99984718299999997</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.97763778999999995</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.97743403399999995</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-E2D3-4296-A994-6028BCA7C4A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$G$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Avg</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="4"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$G$256:$G$284</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.86930238340748101</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.88102165908758401</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.88460668749358495</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.89003388478670897</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.89202145086934403</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.87738719898892903</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.86906933763147098</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.88057417526816495</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.88732187264928797</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.88484370776458698</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.88926474090908902</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.88973183873914197</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.86795404100634499</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.84714753742748805</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.83734596197663402</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.83331070868903701</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.836275244390562</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.84126783726606902</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.85679886708987596</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.871360508827693</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.86388897357483996</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.85447913018620902</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.85336809433987304</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.84881660799376901</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.84366965137814698</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.86177905842341096</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.89314237537229701</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.91341789039406895</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.93252530981451998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-E2D3-4296-A994-6028BCA7C4A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$H$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Max</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$H$256:$H$284</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.95648512070085501</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.96584169962785704</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97274158422510104</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.97949567101443802</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.97930613360656005</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.96521841360192395</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.95752757526352195</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.96634105710920504</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.97560651224526596</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.97375852428944998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.97922958968227602</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.97855527465970804</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.95682045591664</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.92860127630739597</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.91576012792529504</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.91321959984525702</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.91589863590720599</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.92026892727073795</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.94347994983852501</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.95925528055374498</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.94664740896482702</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.93831505992816899</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.93696278464803595</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.92815294760801703</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.92714694217533</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.94948317725167797</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.98187946622557698</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>1.0082725273569899</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>1.0318115950999001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-E2D3-4296-A994-6028BCA7C4A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Data!$I$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Min</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="3"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Data!$I$256:$I$284</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="29"/>
+                <c:pt idx="0">
+                  <c:v>0.78635652423640301</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.811003797137689</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.80005283574268704</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.793622268985409</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.82058557887595096</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.80492859545167295</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.77693657194639498</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.808057277840043</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.81524543918925696</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.78419190432772301</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.81754014643419104</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.81605230761376601</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.77394205347878198</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.773377366803915</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.76218096215121101</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.74906106466134303</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.76129103701470902</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.76442088374168304</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.77041605376106104</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.79575378281934295</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.78479144144763702</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.77234281994212395</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.77526009496288195</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.76798606646928602</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.76666617028200201</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.77653762673303595</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.81087974923663297</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.82836350429461503</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.81870218160221397</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-E2D3-4296-A994-6028BCA7C4A5}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:hiLowLines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:hiLowLines>
+        <c:smooth val="0"/>
+        <c:axId val="500817840"/>
+        <c:axId val="500824400"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="500817840"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="500824400"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="500824400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.1000000000000001"/>
+          <c:min val="0.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="500817840"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1500,20 +2407,536 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>600074</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>152399</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>142874</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1527,6 +2950,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>161925</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1611,6 +3064,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -1646,6 +3116,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1798,15 +3285,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F284"/>
+  <dimension ref="A1:J284"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R1" sqref="R1"/>
+      <selection activeCell="G1" activeCellId="3" sqref="A256:A284 G256:I284 A1 G1:I1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="6" width="9.140625" style="2"/>
+    <col min="7" max="9" width="9.140625" style="3"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1816,42 +3307,54 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4.7288349E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="J2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.5383569999999999E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>4.0513464999999999E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>9.7802830000000007E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2.6284511E-2</v>
       </c>
@@ -1859,7 +3362,7 @@
         <v>4.59158640474933E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1.1359391E-2</v>
       </c>
@@ -1867,7 +3370,7 @@
         <v>7.77858468206169E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>4.0802118999999998E-2</v>
       </c>
@@ -1875,7 +3378,7 @@
         <v>6.8061512750133502E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8.2758855000000006E-2</v>
       </c>
@@ -1883,7 +3386,7 @@
         <v>7.4868152849254799E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>0.100264883</v>
       </c>
@@ -1891,7 +3394,7 @@
         <v>0.146430323590794</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9.6818011999999995E-2</v>
       </c>
@@ -1899,7 +3402,7 @@
         <v>0.25051321087274497</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>5.1855877000000002E-2</v>
       </c>
@@ -1907,7 +3410,7 @@
         <v>2.5858294361391502E-4</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4.4503685000000001E-2</v>
       </c>
@@ -1915,7 +3418,7 @@
         <v>1.39055181870134E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>8.3149387000000005E-2</v>
       </c>
@@ -1923,7 +3426,7 @@
         <v>2.58134481689196E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>0.131626312</v>
       </c>
@@ -3723,7 +5226,7 @@
         <v>0.83102462558326295</v>
       </c>
     </row>
-    <row r="241" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>0.86628519000000004</v>
       </c>
@@ -3731,7 +5234,7 @@
         <v>0.84083454762255205</v>
       </c>
     </row>
-    <row r="242" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>0.90009169</v>
       </c>
@@ -3739,7 +5242,7 @@
         <v>0.85046139508709695</v>
       </c>
     </row>
-    <row r="243" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>0.94216728400000005</v>
       </c>
@@ -3747,7 +5250,7 @@
         <v>0.86168799885588099</v>
       </c>
     </row>
-    <row r="244" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>0.93812612500000003</v>
       </c>
@@ -3755,7 +5258,7 @@
         <v>0.88400747077031105</v>
       </c>
     </row>
-    <row r="245" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>0.9214521</v>
       </c>
@@ -3763,7 +5266,7 @@
         <v>0.90047103552348495</v>
       </c>
     </row>
-    <row r="246" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>0.93242095999999997</v>
       </c>
@@ -3771,7 +5274,7 @@
         <v>0.91131377883543496</v>
       </c>
     </row>
-    <row r="247" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>0.94388222899999996</v>
       </c>
@@ -3779,7 +5282,7 @@
         <v>0.92053571268978696</v>
       </c>
     </row>
-    <row r="248" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>0.92196149000000005</v>
       </c>
@@ -3787,7 +5290,7 @@
         <v>0.92678094359554297</v>
       </c>
     </row>
-    <row r="249" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>0.84037423200000005</v>
       </c>
@@ -3795,7 +5298,7 @@
         <v>0.92477542797560497</v>
       </c>
     </row>
-    <row r="250" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>0.83612931700000004</v>
       </c>
@@ -3803,7 +5306,7 @@
         <v>0.91261012677776299</v>
       </c>
     </row>
-    <row r="251" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>0.87064896300000005</v>
       </c>
@@ -3811,7 +5314,7 @@
         <v>0.90182294762762005</v>
       </c>
     </row>
-    <row r="252" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>0.86867932199999998</v>
       </c>
@@ -3819,7 +5322,7 @@
         <v>0.89402190545121296</v>
       </c>
     </row>
-    <row r="253" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>0.85752368700000003</v>
       </c>
@@ -3827,7 +5330,7 @@
         <v>0.88422643428111303</v>
       </c>
     </row>
-    <row r="254" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>0.90995687199999997</v>
       </c>
@@ -3835,7 +5338,7 @@
         <v>0.87575478794415695</v>
       </c>
     </row>
-    <row r="255" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>0.94889122800000003</v>
       </c>
@@ -3843,501 +5346,763 @@
         <v>0.88604422332483102</v>
       </c>
     </row>
-    <row r="256" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>0.91423574600000002</v>
       </c>
       <c r="C256">
         <v>0.90206704983711805</v>
       </c>
-      <c r="D256">
+      <c r="D256" s="2">
         <v>0.86930238340748101</v>
       </c>
-      <c r="E256">
+      <c r="E256" s="2">
         <v>0.95648512070085501</v>
       </c>
-      <c r="F256">
+      <c r="F256" s="2">
         <v>0.78635652423640301</v>
       </c>
-    </row>
-    <row r="257" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G256" s="3">
+        <v>0.86930238340748101</v>
+      </c>
+      <c r="H256" s="3">
+        <v>0.95648512070085501</v>
+      </c>
+      <c r="I256" s="3">
+        <v>0.78635652423640301</v>
+      </c>
+    </row>
+    <row r="257" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>0.90082181500000003</v>
       </c>
       <c r="C257">
         <v>0.90850205151062702</v>
       </c>
-      <c r="D257">
+      <c r="D257" s="2">
         <v>0.88102165908758401</v>
       </c>
-      <c r="E257">
+      <c r="E257" s="2">
         <v>0.96584169962785704</v>
       </c>
-      <c r="F257">
+      <c r="F257" s="2">
         <v>0.811003797137689</v>
       </c>
-    </row>
-    <row r="258" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G257" s="3">
+        <v>0.88102165908758401</v>
+      </c>
+      <c r="H257" s="3">
+        <v>0.96584169962785704</v>
+      </c>
+      <c r="I257" s="3">
+        <v>0.811003797137689</v>
+      </c>
+    </row>
+    <row r="258" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>0.88898699400000003</v>
       </c>
       <c r="C258">
         <v>0.91336006323761998</v>
       </c>
-      <c r="D258">
+      <c r="D258" s="2">
         <v>0.88460668749358495</v>
       </c>
-      <c r="E258">
+      <c r="E258" s="2">
         <v>0.97274158422510104</v>
       </c>
-      <c r="F258">
+      <c r="F258" s="2">
         <v>0.80005283574268704</v>
       </c>
-    </row>
-    <row r="259" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G258" s="3">
+        <v>0.88460668749358495</v>
+      </c>
+      <c r="H258" s="3">
+        <v>0.97274158422510104</v>
+      </c>
+      <c r="I258" s="3">
+        <v>0.80005283574268704</v>
+      </c>
+    </row>
+    <row r="259" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>0.90907392899999995</v>
       </c>
       <c r="C259">
         <v>0.91810007922630299</v>
       </c>
-      <c r="D259">
+      <c r="D259" s="2">
         <v>0.89003388478670897</v>
       </c>
-      <c r="E259">
+      <c r="E259" s="2">
         <v>0.97949567101443802</v>
       </c>
-      <c r="F259">
+      <c r="F259" s="2">
         <v>0.793622268985409</v>
       </c>
-    </row>
-    <row r="260" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G259" s="3">
+        <v>0.89003388478670897</v>
+      </c>
+      <c r="H259" s="3">
+        <v>0.97949567101443802</v>
+      </c>
+      <c r="I259" s="3">
+        <v>0.793622268985409</v>
+      </c>
+    </row>
+    <row r="260" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>0.88326484900000002</v>
       </c>
       <c r="C260">
         <v>0.91853770013064195</v>
       </c>
-      <c r="D260">
+      <c r="D260" s="2">
         <v>0.89202145086934403</v>
       </c>
-      <c r="E260">
+      <c r="E260" s="2">
         <v>0.97930613360656005</v>
       </c>
-      <c r="F260">
+      <c r="F260" s="2">
         <v>0.82058557887595096</v>
       </c>
-    </row>
-    <row r="261" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G260" s="3">
+        <v>0.89202145086934403</v>
+      </c>
+      <c r="H260" s="3">
+        <v>0.97930613360656005</v>
+      </c>
+      <c r="I260" s="3">
+        <v>0.82058557887595096</v>
+      </c>
+    </row>
+    <row r="261" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>0.878408666</v>
       </c>
       <c r="C261">
         <v>0.91031512896413602</v>
       </c>
-      <c r="D261">
+      <c r="D261" s="2">
         <v>0.87738719898892903</v>
       </c>
-      <c r="E261">
+      <c r="E261" s="2">
         <v>0.96521841360192395</v>
       </c>
-      <c r="F261">
+      <c r="F261" s="2">
         <v>0.80492859545167295</v>
       </c>
-    </row>
-    <row r="262" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G261" s="3">
+        <v>0.87738719898892903</v>
+      </c>
+      <c r="H261" s="3">
+        <v>0.96521841360192395</v>
+      </c>
+      <c r="I261" s="3">
+        <v>0.80492859545167295</v>
+      </c>
+    </row>
+    <row r="262" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>0.94187862899999997</v>
       </c>
       <c r="C262">
         <v>0.90601178236823898</v>
       </c>
-      <c r="D262">
+      <c r="D262" s="2">
         <v>0.86906933763147098</v>
       </c>
-      <c r="E262">
+      <c r="E262" s="2">
         <v>0.95752757526352195</v>
       </c>
-      <c r="F262">
+      <c r="F262" s="2">
         <v>0.77693657194639498</v>
       </c>
-    </row>
-    <row r="263" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G262" s="3">
+        <v>0.86906933763147098</v>
+      </c>
+      <c r="H262" s="3">
+        <v>0.95752757526352195</v>
+      </c>
+      <c r="I262" s="3">
+        <v>0.77693657194639498</v>
+      </c>
+    </row>
+    <row r="263" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>0.93214928500000005</v>
       </c>
       <c r="C263">
         <v>0.91210512740358796</v>
       </c>
-      <c r="D263">
+      <c r="D263" s="2">
         <v>0.88057417526816495</v>
       </c>
-      <c r="E263">
+      <c r="E263" s="2">
         <v>0.96634105710920504</v>
       </c>
-      <c r="F263">
+      <c r="F263" s="2">
         <v>0.808057277840043</v>
       </c>
-    </row>
-    <row r="264" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G263" s="3">
+        <v>0.88057417526816495</v>
+      </c>
+      <c r="H263" s="3">
+        <v>0.96634105710920504</v>
+      </c>
+      <c r="I263" s="3">
+        <v>0.808057277840043</v>
+      </c>
+    </row>
+    <row r="264" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>0.90046524299999997</v>
       </c>
       <c r="C264">
         <v>0.91843304867980202</v>
       </c>
-      <c r="D264">
+      <c r="D264" s="2">
         <v>0.88732187264928797</v>
       </c>
-      <c r="E264">
+      <c r="E264" s="2">
         <v>0.97560651224526596</v>
       </c>
-      <c r="F264">
+      <c r="F264" s="2">
         <v>0.81524543918925696</v>
       </c>
-    </row>
-    <row r="265" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G264" s="3">
+        <v>0.88732187264928797</v>
+      </c>
+      <c r="H264" s="3">
+        <v>0.97560651224526596</v>
+      </c>
+      <c r="I264" s="3">
+        <v>0.81524543918925696</v>
+      </c>
+    </row>
+    <row r="265" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>0.90875131600000003</v>
       </c>
       <c r="C265">
         <v>0.91782201683522402</v>
       </c>
-      <c r="D265">
+      <c r="D265" s="2">
         <v>0.88484370776458698</v>
       </c>
-      <c r="E265">
+      <c r="E265" s="2">
         <v>0.97375852428944998</v>
       </c>
-      <c r="F265">
+      <c r="F265" s="2">
         <v>0.78419190432772301</v>
       </c>
-    </row>
-    <row r="266" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G265" s="3">
+        <v>0.88484370776458698</v>
+      </c>
+      <c r="H265" s="3">
+        <v>0.97375852428944998</v>
+      </c>
+      <c r="I265" s="3">
+        <v>0.78419190432772301</v>
+      </c>
+    </row>
+    <row r="266" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>0.87526742999999996</v>
       </c>
       <c r="C266">
         <v>0.92176140843629994</v>
       </c>
-      <c r="D266">
+      <c r="D266" s="2">
         <v>0.81788975953176202</v>
       </c>
-      <c r="E266">
+      <c r="E266" s="2">
         <v>0.97922958968227602</v>
       </c>
-      <c r="F266">
+      <c r="F266" s="2">
         <v>-0.538234886637462</v>
       </c>
-    </row>
-    <row r="267" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G266" s="3">
+        <v>0.88926474090908902</v>
+      </c>
+      <c r="H266" s="3">
+        <v>0.97922958968227602</v>
+      </c>
+      <c r="I266" s="3">
+        <v>0.81754014643419104</v>
+      </c>
+    </row>
+    <row r="267" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>0.84062892700000003</v>
       </c>
       <c r="C267">
         <v>0.92187870669592298</v>
       </c>
-      <c r="D267">
+      <c r="D267" s="2">
         <v>0.88973183873914197</v>
       </c>
-      <c r="E267">
+      <c r="E267" s="2">
         <v>0.97855527465970804</v>
       </c>
-      <c r="F267">
+      <c r="F267" s="2">
         <v>0.81605230761376601</v>
       </c>
-    </row>
-    <row r="268" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G267" s="3">
+        <v>0.88973183873914197</v>
+      </c>
+      <c r="H267" s="3">
+        <v>0.97855527465970804</v>
+      </c>
+      <c r="I267" s="3">
+        <v>0.81605230761376601</v>
+      </c>
+    </row>
+    <row r="268" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>0.80069277000000005</v>
       </c>
       <c r="C268">
         <v>0.90875395251479996</v>
       </c>
-      <c r="D268">
+      <c r="D268" s="2">
         <v>0.86795404100634499</v>
       </c>
-      <c r="E268">
+      <c r="E268" s="2">
         <v>0.95682045591664</v>
       </c>
-      <c r="F268">
+      <c r="F268" s="2">
         <v>0.77394205347878198</v>
       </c>
-    </row>
-    <row r="269" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G268" s="3">
+        <v>0.86795404100634499</v>
+      </c>
+      <c r="H268" s="3">
+        <v>0.95682045591664</v>
+      </c>
+      <c r="I268" s="3">
+        <v>0.77394205347878198</v>
+      </c>
+    </row>
+    <row r="269" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>0.840645906</v>
       </c>
       <c r="C269">
         <v>0.89106325838280598</v>
       </c>
-      <c r="D269">
+      <c r="D269" s="2">
         <v>0.84714753742748805</v>
       </c>
-      <c r="E269">
+      <c r="E269" s="2">
         <v>0.92860127630739597</v>
       </c>
-      <c r="F269">
+      <c r="F269" s="2">
         <v>0.773377366803915</v>
       </c>
-    </row>
-    <row r="270" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G269" s="3">
+        <v>0.84714753742748805</v>
+      </c>
+      <c r="H269" s="3">
+        <v>0.92860127630739597</v>
+      </c>
+      <c r="I269" s="3">
+        <v>0.773377366803915</v>
+      </c>
+    </row>
+    <row r="270" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>0.89691649399999995</v>
       </c>
       <c r="C270">
         <v>0.88309617131567997</v>
       </c>
-      <c r="D270">
+      <c r="D270" s="2">
         <v>0.83734596197663402</v>
       </c>
-      <c r="E270">
+      <c r="E270" s="2">
         <v>0.91576012792529504</v>
       </c>
-      <c r="F270">
+      <c r="F270" s="2">
         <v>0.76218096215121101</v>
       </c>
-    </row>
-    <row r="271" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G270" s="3">
+        <v>0.83734596197663402</v>
+      </c>
+      <c r="H270" s="3">
+        <v>0.91576012792529504</v>
+      </c>
+      <c r="I270" s="3">
+        <v>0.76218096215121101</v>
+      </c>
+    </row>
+    <row r="271" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>0.88774747899999995</v>
       </c>
       <c r="C271">
         <v>0.88190656574279902</v>
       </c>
-      <c r="D271">
+      <c r="D271" s="2">
         <v>0.83331070868903701</v>
       </c>
-      <c r="E271">
+      <c r="E271" s="2">
         <v>0.91321959984525702</v>
       </c>
-      <c r="F271">
+      <c r="F271" s="2">
         <v>0.74906106466134303</v>
       </c>
-    </row>
-    <row r="272" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G271" s="3">
+        <v>0.83331070868903701</v>
+      </c>
+      <c r="H271" s="3">
+        <v>0.91321959984525702</v>
+      </c>
+      <c r="I271" s="3">
+        <v>0.74906106466134303</v>
+      </c>
+    </row>
+    <row r="272" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>0.86098753699999997</v>
       </c>
       <c r="C272">
         <v>0.88419099531437195</v>
       </c>
-      <c r="D272">
+      <c r="D272" s="2">
         <v>0.836275244390562</v>
       </c>
-      <c r="E272">
+      <c r="E272" s="2">
         <v>0.91589863590720599</v>
       </c>
-      <c r="F272">
+      <c r="F272" s="2">
         <v>0.76129103701470902</v>
       </c>
-    </row>
-    <row r="273" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G272" s="3">
+        <v>0.836275244390562</v>
+      </c>
+      <c r="H272" s="3">
+        <v>0.91589863590720599</v>
+      </c>
+      <c r="I272" s="3">
+        <v>0.76129103701470902</v>
+      </c>
+    </row>
+    <row r="273" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>0.90881923499999995</v>
       </c>
       <c r="C273">
         <v>0.887591545266742</v>
       </c>
-      <c r="D273">
+      <c r="D273" s="2">
         <v>0.84126783726606902</v>
       </c>
-      <c r="E273">
+      <c r="E273" s="2">
         <v>0.92026892727073795</v>
       </c>
-      <c r="F273">
+      <c r="F273" s="2">
         <v>0.76442088374168304</v>
       </c>
-    </row>
-    <row r="274" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G273" s="3">
+        <v>0.84126783726606902</v>
+      </c>
+      <c r="H273" s="3">
+        <v>0.92026892727073795</v>
+      </c>
+      <c r="I273" s="3">
+        <v>0.76442088374168304</v>
+      </c>
+    </row>
+    <row r="274" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>0.91413386799999996</v>
       </c>
       <c r="C274">
         <v>0.90328642412808102</v>
       </c>
-      <c r="D274">
+      <c r="D274" s="2">
         <v>0.85679886708987596</v>
       </c>
-      <c r="E274">
+      <c r="E274" s="2">
         <v>0.94347994983852501</v>
       </c>
-      <c r="F274">
+      <c r="F274" s="2">
         <v>0.77041605376106104</v>
       </c>
-    </row>
-    <row r="275" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G274" s="3">
+        <v>0.85679886708987596</v>
+      </c>
+      <c r="H274" s="3">
+        <v>0.94347994983852501</v>
+      </c>
+      <c r="I274" s="3">
+        <v>0.77041605376106104</v>
+      </c>
+    </row>
+    <row r="275" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>0.838183856</v>
       </c>
       <c r="C275">
         <v>0.91391252630247899</v>
       </c>
-      <c r="D275">
+      <c r="D275" s="2">
         <v>0.871360508827693</v>
       </c>
-      <c r="E275">
+      <c r="E275" s="2">
         <v>0.95925528055374498</v>
       </c>
-      <c r="F275">
+      <c r="F275" s="2">
         <v>0.79575378281934295</v>
       </c>
-    </row>
-    <row r="276" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G275" s="3">
+        <v>0.871360508827693</v>
+      </c>
+      <c r="H275" s="3">
+        <v>0.95925528055374498</v>
+      </c>
+      <c r="I275" s="3">
+        <v>0.79575378281934295</v>
+      </c>
+    </row>
+    <row r="276" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>0.84893197899999995</v>
       </c>
       <c r="C276">
         <v>0.90633773471140799</v>
       </c>
-      <c r="D276">
+      <c r="D276" s="2">
         <v>0.86388897357483996</v>
       </c>
-      <c r="E276">
+      <c r="E276" s="2">
         <v>0.94664740896482702</v>
       </c>
-      <c r="F276">
+      <c r="F276" s="2">
         <v>0.78479144144763702</v>
       </c>
-    </row>
-    <row r="277" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G276" s="3">
+        <v>0.86388897357483996</v>
+      </c>
+      <c r="H276" s="3">
+        <v>0.94664740896482702</v>
+      </c>
+      <c r="I276" s="3">
+        <v>0.78479144144763702</v>
+      </c>
+    </row>
+    <row r="277" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>0.85468808399999996</v>
       </c>
       <c r="C277">
         <v>0.90143436343377004</v>
       </c>
-      <c r="D277">
+      <c r="D277" s="2">
         <v>0.85447913018620902</v>
       </c>
-      <c r="E277">
+      <c r="E277" s="2">
         <v>0.93831505992816899</v>
       </c>
-      <c r="F277">
+      <c r="F277" s="2">
         <v>0.77234281994212395</v>
       </c>
-    </row>
-    <row r="278" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G277" s="3">
+        <v>0.85447913018620902</v>
+      </c>
+      <c r="H277" s="3">
+        <v>0.93831505992816899</v>
+      </c>
+      <c r="I277" s="3">
+        <v>0.77234281994212395</v>
+      </c>
+    </row>
+    <row r="278" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>0.86777939999999998</v>
       </c>
       <c r="C278">
         <v>0.90104689840336505</v>
       </c>
-      <c r="D278">
+      <c r="D278" s="2">
         <v>0.85336809433987304</v>
       </c>
-      <c r="E278">
+      <c r="E278" s="2">
         <v>0.93696278464803595</v>
       </c>
-      <c r="F278">
+      <c r="F278" s="2">
         <v>0.77526009496288195</v>
       </c>
-    </row>
-    <row r="279" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G278" s="3">
+        <v>0.85336809433987304</v>
+      </c>
+      <c r="H278" s="3">
+        <v>0.93696278464803595</v>
+      </c>
+      <c r="I278" s="3">
+        <v>0.77526009496288195</v>
+      </c>
+    </row>
+    <row r="279" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>0.90944748200000003</v>
       </c>
       <c r="C279">
         <v>0.89575875293296303</v>
       </c>
-      <c r="D279">
+      <c r="D279" s="2">
         <v>0.84881660799376901</v>
       </c>
-      <c r="E279">
+      <c r="E279" s="2">
         <v>0.92815294760801703</v>
       </c>
-      <c r="F279">
+      <c r="F279" s="2">
         <v>0.76798606646928602</v>
       </c>
-    </row>
-    <row r="280" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G279" s="3">
+        <v>0.84881660799376901</v>
+      </c>
+      <c r="H279" s="3">
+        <v>0.92815294760801703</v>
+      </c>
+      <c r="I279" s="3">
+        <v>0.76798606646928602</v>
+      </c>
+    </row>
+    <row r="280" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>0.94223520199999999</v>
       </c>
       <c r="C280">
         <v>0.89558115943773398</v>
       </c>
-      <c r="D280">
+      <c r="D280" s="2">
         <v>0.84366965137814698</v>
       </c>
-      <c r="E280">
+      <c r="E280" s="2">
         <v>0.92714694217533</v>
       </c>
-      <c r="F280">
+      <c r="F280" s="2">
         <v>0.76666617028200201</v>
       </c>
-    </row>
-    <row r="281" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G280" s="3">
+        <v>0.84366965137814698</v>
+      </c>
+      <c r="H280" s="3">
+        <v>0.92714694217533</v>
+      </c>
+      <c r="I280" s="3">
+        <v>0.76666617028200201</v>
+      </c>
+    </row>
+    <row r="281" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>0.99984718299999997</v>
       </c>
       <c r="C281">
         <v>0.91064523092445004</v>
       </c>
-      <c r="D281">
+      <c r="D281" s="2">
         <v>0.86177905842341096</v>
       </c>
-      <c r="E281">
+      <c r="E281" s="2">
         <v>0.94948317725167797</v>
       </c>
-      <c r="F281">
+      <c r="F281" s="2">
         <v>0.77653762673303595</v>
       </c>
-    </row>
-    <row r="282" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G281" s="3">
+        <v>0.86177905842341096</v>
+      </c>
+      <c r="H281" s="3">
+        <v>0.94948317725167797</v>
+      </c>
+      <c r="I281" s="3">
+        <v>0.77653762673303595</v>
+      </c>
+    </row>
+    <row r="282" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>0.97763778999999995</v>
       </c>
       <c r="C282">
         <v>0.931694567839915</v>
       </c>
-      <c r="D282">
+      <c r="D282" s="2">
         <v>0.89314237537229701</v>
       </c>
-      <c r="E282">
+      <c r="E282" s="2">
         <v>0.98187946622557698</v>
       </c>
-      <c r="F282">
+      <c r="F282" s="2">
         <v>0.81087974923663297</v>
       </c>
-    </row>
-    <row r="283" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G282" s="3">
+        <v>0.89314237537229701</v>
+      </c>
+      <c r="H282" s="3">
+        <v>0.98187946622557698</v>
+      </c>
+      <c r="I282" s="3">
+        <v>0.81087974923663297</v>
+      </c>
+    </row>
+    <row r="283" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>0.97743403399999995</v>
       </c>
       <c r="C283">
         <v>0.94845612003250002</v>
       </c>
-      <c r="D283">
+      <c r="D283" s="2">
         <v>0.91341789039406895</v>
       </c>
-      <c r="E283">
+      <c r="E283" s="2">
         <v>1.0082725273569899</v>
       </c>
-      <c r="F283">
+      <c r="F283" s="2">
         <v>0.82836350429461503</v>
       </c>
-    </row>
-    <row r="284" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G283" s="3">
+        <v>0.91341789039406895</v>
+      </c>
+      <c r="H283" s="3">
+        <v>1.0082725273569899</v>
+      </c>
+      <c r="I283" s="3">
+        <v>0.82836350429461503</v>
+      </c>
+    </row>
+    <row r="284" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>1</v>
       </c>
       <c r="C284">
         <v>0.96311776009783501</v>
       </c>
-      <c r="D284">
+      <c r="D284" s="2">
         <v>0.93252530981451998</v>
       </c>
-      <c r="E284">
+      <c r="E284" s="2">
         <v>1.0318115950999001</v>
       </c>
-      <c r="F284">
+      <c r="F284" s="2">
+        <v>0.81870218160221397</v>
+      </c>
+      <c r="G284" s="3">
+        <v>0.93252530981451998</v>
+      </c>
+      <c r="H284" s="3">
+        <v>1.0318115950999001</v>
+      </c>
+      <c r="I284" s="3">
         <v>0.81870218160221397</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -4346,7 +6111,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="U11" sqref="U11"/>
+      <selection activeCell="R25" sqref="R25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>